<commit_message>
Update comparison of MQ PEAKS and pyBinder
</commit_message>
<xml_diff>
--- a/Comparison of MaxQuant PEAKS and pyBinder.xlsx
+++ b/Comparison of MaxQuant PEAKS and pyBinder.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\SDL3\Documents\GitHub\pyBinder\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{781B04C8-BABA-4DC1-8039-D1F2EC3E6DD5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6783F862-32D9-4A04-8679-F7B63B548DAC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{3460C30C-307E-4DAD-885D-85ED9727F4C1}"/>
+    <workbookView xWindow="-38520" yWindow="-1680" windowWidth="38640" windowHeight="21120" activeTab="1" xr2:uid="{3460C30C-307E-4DAD-885D-85ED9727F4C1}"/>
   </bookViews>
   <sheets>
     <sheet name="summary" sheetId="1" r:id="rId1"/>
@@ -34,7 +34,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="244" uniqueCount="120">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="247" uniqueCount="124">
   <si>
     <t>Raw file</t>
   </si>
@@ -345,12 +345,6 @@
     <t>Peptide features (Isoptope patterns)</t>
   </si>
   <si>
-    <t>Peptide features sequenced z={1-6} (Isoptope patterns sequenced, z&gt;1)</t>
-  </si>
-  <si>
-    <t>Peptide features z={1-6}</t>
-  </si>
-  <si>
     <t>Data acquisition</t>
   </si>
   <si>
@@ -363,15 +357,9 @@
     <t>Quantifies selectivity of MS/MS identified?</t>
   </si>
   <si>
-    <t>44869, across all replicates</t>
-  </si>
-  <si>
     <t>Yes, and p-value</t>
   </si>
   <si>
-    <t>Filtered output missing</t>
-  </si>
-  <si>
     <t>Relevant items from MaxQuant outputs</t>
   </si>
   <si>
@@ -390,17 +378,44 @@
     <t>*Analysis of CDE would require custom written code, as done in this work</t>
   </si>
   <si>
-    <t>Post-analysis</t>
-  </si>
-  <si>
     <t>"Sequencing fidelity" (MS/MS identified / Peptide features sequenced</t>
+  </si>
+  <si>
+    <t>Post-analysis of PEAKS output</t>
+  </si>
+  <si>
+    <t>*Not a direct output</t>
+  </si>
+  <si>
+    <t>Isotope patterns, z={2-6}*</t>
+  </si>
+  <si>
+    <t>Peptide features z={2-6}</t>
+  </si>
+  <si>
+    <t>Peptide features sequenced z={2-6}</t>
+  </si>
+  <si>
+    <t>"Feature coverage" = Isotope patterns sequenced [%]</t>
+  </si>
+  <si>
+    <t>Average:</t>
+  </si>
+  <si>
+    <t>Multiply averages</t>
+  </si>
+  <si>
+    <t>44869, matched between runs, across all replicates</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="18" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="168" formatCode="0.0%"/>
+  </numFmts>
+  <fonts count="19" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -535,6 +550,13 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="14"/>
+      <color theme="1"/>
+      <name val="Aptos Narrow"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="42">
     <fill>
@@ -748,12 +770,6 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFFF9999"/>
-        <bgColor indexed="64"/>
-      </patternFill>
-    </fill>
-    <fill>
-      <patternFill patternType="solid">
         <fgColor theme="0" tint="-0.14999847407452621"/>
         <bgColor indexed="64"/>
       </patternFill>
@@ -767,6 +783,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC1C1"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -962,85 +984,87 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="36" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="37" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="34" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="16" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="38" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
+    <xf numFmtId="9" fontId="0" fillId="39" borderId="0" xfId="42" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="39" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="9" fontId="0" fillId="39" borderId="0" xfId="42" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="16" fillId="41" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="35" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1"/>
-    <xf numFmtId="0" fontId="16" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
-      <alignment horizontal="left"/>
-    </xf>
-    <xf numFmtId="9" fontId="0" fillId="40" borderId="0" xfId="42" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="10" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="11" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="right"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="40" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="16" fillId="33" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="0" fillId="35" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="36" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="38" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="37" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="18" fillId="40" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="41" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center" wrapText="1"/>
+    <xf numFmtId="0" fontId="18" fillId="34" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="9" fontId="0" fillId="40" borderId="0" xfId="42" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="16" fillId="39" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="1" fontId="16" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="168" fontId="16" fillId="39" borderId="0" xfId="42" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
+      <alignment horizontal="right"/>
+    </xf>
+    <xf numFmtId="10" fontId="16" fillId="39" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
   </cellXfs>
@@ -1093,6 +1117,7 @@
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
   <colors>
     <mruColors>
+      <color rgb="FFFFC1C1"/>
       <color rgb="FFFF9999"/>
     </mruColors>
   </colors>
@@ -1430,9 +1455,9 @@
       <selection activeCell="AQ1" sqref="AQ1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <sheetData>
-    <row r="1" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1623,7 +1648,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="2" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>63</v>
       </c>
@@ -1793,7 +1818,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>71</v>
       </c>
@@ -1963,7 +1988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>73</v>
       </c>
@@ -2133,7 +2158,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>75</v>
       </c>
@@ -2303,7 +2328,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="6" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>77</v>
       </c>
@@ -2473,7 +2498,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>79</v>
       </c>
@@ -2643,7 +2668,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="8" spans="1:63" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:63" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>81</v>
       </c>
@@ -2739,103 +2764,104 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E02F34AE-AD65-4756-A0EC-9D42D86747E8}">
-  <dimension ref="A1:S49"/>
+  <dimension ref="A1:S53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScale="115" zoomScaleNormal="115" workbookViewId="0">
-      <selection activeCell="Q17" sqref="Q17"/>
+      <selection activeCell="A2" sqref="A2:S34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="18" customWidth="1"/>
+    <col min="1" max="1" width="15.5546875" customWidth="1"/>
     <col min="2" max="3" width="18" hidden="1" customWidth="1"/>
-    <col min="6" max="6" width="11.42578125" customWidth="1"/>
-    <col min="7" max="7" width="13.5703125" hidden="1" customWidth="1"/>
-    <col min="8" max="8" width="11.140625" hidden="1" customWidth="1"/>
-    <col min="9" max="9" width="11.42578125" hidden="1" customWidth="1"/>
-    <col min="10" max="10" width="13.140625" style="2" hidden="1" customWidth="1"/>
-    <col min="11" max="11" width="15.28515625" hidden="1" customWidth="1"/>
-    <col min="12" max="12" width="14.85546875" customWidth="1"/>
-    <col min="13" max="13" width="10.140625" customWidth="1"/>
-    <col min="14" max="14" width="20.7109375" customWidth="1"/>
-    <col min="15" max="15" width="15.7109375" customWidth="1"/>
-    <col min="16" max="16" width="19.5703125" customWidth="1"/>
-    <col min="17" max="17" width="20.28515625" customWidth="1"/>
-    <col min="18" max="18" width="27.7109375" customWidth="1"/>
-    <col min="19" max="19" width="17.140625" customWidth="1"/>
+    <col min="4" max="4" width="7.44140625" customWidth="1"/>
+    <col min="6" max="6" width="9.33203125" customWidth="1"/>
+    <col min="7" max="7" width="13.5546875" hidden="1" customWidth="1"/>
+    <col min="8" max="8" width="11.109375" hidden="1" customWidth="1"/>
+    <col min="9" max="9" width="11.44140625" hidden="1" customWidth="1"/>
+    <col min="10" max="10" width="13.109375" style="2" hidden="1" customWidth="1"/>
+    <col min="11" max="11" width="15.33203125" hidden="1" customWidth="1"/>
+    <col min="12" max="12" width="10" customWidth="1"/>
+    <col min="13" max="13" width="9.5546875" customWidth="1"/>
+    <col min="14" max="14" width="15.109375" customWidth="1"/>
+    <col min="15" max="15" width="14.77734375" customWidth="1"/>
+    <col min="16" max="16" width="17.5546875" customWidth="1"/>
+    <col min="17" max="17" width="20.33203125" customWidth="1"/>
+    <col min="18" max="18" width="27.6640625" customWidth="1"/>
+    <col min="19" max="19" width="17.109375" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A1" s="21"/>
-      <c r="B1" s="21"/>
-      <c r="C1" s="21"/>
-      <c r="D1" s="21"/>
-      <c r="E1" s="21"/>
-      <c r="F1" s="21"/>
-      <c r="G1" s="21"/>
-      <c r="H1" s="21"/>
-      <c r="I1" s="21"/>
-      <c r="J1" s="25"/>
-      <c r="K1" s="21"/>
-      <c r="L1" s="21"/>
-      <c r="M1" s="21"/>
-      <c r="N1" s="21"/>
-      <c r="O1" s="21"/>
-      <c r="P1" s="21"/>
-      <c r="Q1" s="21"/>
-      <c r="R1" s="21"/>
-      <c r="S1" s="21"/>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A2" s="21"/>
-      <c r="B2" s="21"/>
-      <c r="C2" s="21"/>
-      <c r="D2" s="21"/>
-      <c r="E2" s="21"/>
-      <c r="F2" s="21"/>
-      <c r="G2" s="21"/>
-      <c r="H2" s="21"/>
-      <c r="I2" s="21"/>
-      <c r="J2" s="25"/>
-      <c r="K2" s="21"/>
-      <c r="L2" s="21"/>
-      <c r="M2" s="21"/>
-      <c r="N2" s="21"/>
-      <c r="O2" s="21"/>
-      <c r="P2" s="34" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q2" s="34"/>
-      <c r="R2" s="34"/>
-      <c r="S2" s="21"/>
-    </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A3" s="21"/>
-      <c r="D3" s="17" t="s">
-        <v>105</v>
-      </c>
-      <c r="E3" s="17"/>
-      <c r="F3" s="6" t="s">
-        <v>112</v>
-      </c>
-      <c r="G3" s="6"/>
-      <c r="H3" s="6"/>
-      <c r="I3" s="6"/>
-      <c r="J3" s="6"/>
-      <c r="K3" s="6"/>
-      <c r="L3" s="6"/>
-      <c r="M3" s="6"/>
-      <c r="N3" s="6"/>
-      <c r="O3" s="6"/>
-      <c r="P3" s="7" t="s">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A1" s="9"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
+      <c r="G1" s="9"/>
+      <c r="H1" s="9"/>
+      <c r="I1" s="9"/>
+      <c r="J1" s="13"/>
+      <c r="K1" s="9"/>
+      <c r="L1" s="9"/>
+      <c r="M1" s="9"/>
+      <c r="N1" s="9"/>
+      <c r="O1" s="9"/>
+      <c r="P1" s="9"/>
+      <c r="Q1" s="9"/>
+      <c r="R1" s="9"/>
+      <c r="S1" s="9"/>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A2" s="9"/>
+      <c r="B2" s="9"/>
+      <c r="C2" s="9"/>
+      <c r="D2" s="9"/>
+      <c r="E2" s="9"/>
+      <c r="F2" s="9"/>
+      <c r="G2" s="9"/>
+      <c r="H2" s="9"/>
+      <c r="I2" s="9"/>
+      <c r="J2" s="13"/>
+      <c r="K2" s="9"/>
+      <c r="L2" s="9"/>
+      <c r="M2" s="9"/>
+      <c r="N2" s="9"/>
+      <c r="O2" s="9"/>
+      <c r="P2" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q2" s="26"/>
+      <c r="R2" s="26"/>
+      <c r="S2" s="9"/>
+    </row>
+    <row r="3" spans="1:19" ht="18" x14ac:dyDescent="0.35">
+      <c r="A3" s="9"/>
+      <c r="D3" s="29" t="s">
+        <v>103</v>
+      </c>
+      <c r="E3" s="29"/>
+      <c r="F3" s="28" t="s">
+        <v>108</v>
+      </c>
+      <c r="G3" s="28"/>
+      <c r="H3" s="28"/>
+      <c r="I3" s="28"/>
+      <c r="J3" s="28"/>
+      <c r="K3" s="28"/>
+      <c r="L3" s="28"/>
+      <c r="M3" s="28"/>
+      <c r="N3" s="28"/>
+      <c r="O3" s="28"/>
+      <c r="P3" s="30" t="s">
         <v>96</v>
       </c>
-      <c r="Q3" s="7"/>
-      <c r="R3" s="7"/>
-      <c r="S3" s="21"/>
-    </row>
-    <row r="4" spans="1:19" ht="48" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A4" s="22" t="s">
+      <c r="Q3" s="30"/>
+      <c r="R3" s="30"/>
+      <c r="S3" s="9"/>
+    </row>
+    <row r="4" spans="1:19" ht="48" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A4" s="10" t="s">
         <v>0</v>
       </c>
       <c r="B4" t="s">
@@ -2844,53 +2870,55 @@
       <c r="C4" t="s">
         <v>8</v>
       </c>
-      <c r="D4" s="23" t="s">
+      <c r="D4" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="E4" s="32" t="s">
+      <c r="E4" s="20" t="s">
         <v>19</v>
       </c>
-      <c r="F4" s="28" t="s">
-        <v>113</v>
-      </c>
-      <c r="G4" s="28" t="s">
+      <c r="F4" s="16" t="s">
+        <v>109</v>
+      </c>
+      <c r="G4" s="16" t="s">
         <v>83</v>
       </c>
-      <c r="H4" s="28" t="s">
+      <c r="H4" s="16" t="s">
         <v>35</v>
       </c>
-      <c r="I4" s="28" t="s">
+      <c r="I4" s="16" t="s">
         <v>36</v>
       </c>
-      <c r="J4" s="28" t="s">
+      <c r="J4" s="16" t="s">
         <v>37</v>
       </c>
-      <c r="K4" s="31" t="s">
+      <c r="K4" s="19" t="s">
         <v>38</v>
       </c>
-      <c r="L4" s="28" t="s">
+      <c r="L4" s="16" t="s">
         <v>39</v>
       </c>
-      <c r="M4" s="29"/>
-      <c r="N4" s="28" t="s">
+      <c r="M4" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="N4" s="16" t="s">
         <v>41</v>
       </c>
-      <c r="O4" s="28" t="s">
+      <c r="O4" s="16" t="s">
         <v>42</v>
       </c>
-      <c r="P4" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q4" s="28" t="s">
+      <c r="P4" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q4" s="16" t="s">
         <v>101</v>
       </c>
-      <c r="R4" s="28" t="s">
+      <c r="R4" s="16" t="s">
         <v>100</v>
       </c>
-      <c r="S4" s="21"/>
-    </row>
-    <row r="5" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A5" s="21" t="s">
+      <c r="S4" s="9"/>
+    </row>
+    <row r="5" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A5" s="9" t="s">
         <v>75</v>
       </c>
       <c r="B5" t="s">
@@ -2899,13 +2927,13 @@
       <c r="C5" t="s">
         <v>68</v>
       </c>
-      <c r="D5" s="21">
+      <c r="D5" s="9">
         <v>13262</v>
       </c>
-      <c r="E5" s="33">
+      <c r="E5" s="21">
         <v>13552</v>
       </c>
-      <c r="F5" s="8">
+      <c r="F5" s="23">
         <v>5</v>
       </c>
       <c r="G5">
@@ -2923,31 +2951,31 @@
       <c r="K5">
         <v>96</v>
       </c>
-      <c r="L5" s="23">
+      <c r="L5" s="11">
         <v>173621</v>
       </c>
-      <c r="M5" s="19" t="s">
-        <v>111</v>
-      </c>
-      <c r="N5" s="23">
+      <c r="M5" s="11">
+        <v>122844</v>
+      </c>
+      <c r="N5" s="11">
         <v>2753</v>
       </c>
-      <c r="O5" s="21">
+      <c r="O5" s="9">
         <v>1.7</v>
       </c>
-      <c r="P5" s="23" t="s">
+      <c r="P5" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="Q5" s="10" t="s">
+      <c r="Q5" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="R5" s="10" t="s">
+      <c r="R5" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="S5" s="21"/>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A6" s="21" t="s">
+      <c r="S5" s="9"/>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A6" s="9" t="s">
         <v>77</v>
       </c>
       <c r="B6" t="s">
@@ -2956,13 +2984,13 @@
       <c r="C6" t="s">
         <v>68</v>
       </c>
-      <c r="D6" s="21">
+      <c r="D6" s="9">
         <v>14152</v>
       </c>
-      <c r="E6" s="33">
+      <c r="E6" s="21">
         <v>10530</v>
       </c>
-      <c r="F6" s="8">
+      <c r="F6" s="23">
         <v>23</v>
       </c>
       <c r="G6">
@@ -2980,29 +3008,31 @@
       <c r="K6">
         <v>96</v>
       </c>
-      <c r="L6" s="23">
+      <c r="L6" s="11">
         <v>176040</v>
       </c>
-      <c r="M6" s="19"/>
-      <c r="N6" s="23">
+      <c r="M6" s="11">
+        <v>122738</v>
+      </c>
+      <c r="N6" s="11">
         <v>1988</v>
       </c>
-      <c r="O6" s="21">
+      <c r="O6" s="9">
         <v>1.2</v>
       </c>
-      <c r="P6" s="23" t="s">
+      <c r="P6" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="Q6" s="10" t="s">
+      <c r="Q6" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="R6" s="10" t="s">
+      <c r="R6" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="S6" s="21"/>
-    </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A7" s="21" t="s">
+      <c r="S6" s="9"/>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A7" s="9" t="s">
         <v>79</v>
       </c>
       <c r="B7" t="s">
@@ -3011,13 +3041,13 @@
       <c r="C7" t="s">
         <v>68</v>
       </c>
-      <c r="D7" s="21">
+      <c r="D7" s="9">
         <v>15369</v>
       </c>
-      <c r="E7" s="33">
+      <c r="E7" s="21">
         <v>6392</v>
       </c>
-      <c r="F7" s="8">
+      <c r="F7" s="23">
         <v>2</v>
       </c>
       <c r="G7">
@@ -3035,29 +3065,31 @@
       <c r="K7">
         <v>96</v>
       </c>
-      <c r="L7" s="23">
+      <c r="L7" s="11">
         <v>196096</v>
       </c>
-      <c r="M7" s="19"/>
-      <c r="N7" s="23">
+      <c r="M7" s="11">
+        <v>137365</v>
+      </c>
+      <c r="N7" s="11">
         <v>1341</v>
       </c>
-      <c r="O7" s="21">
+      <c r="O7" s="9">
         <v>0.75</v>
       </c>
-      <c r="P7" s="23" t="s">
+      <c r="P7" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="Q7" s="10" t="s">
+      <c r="Q7" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="R7" s="10" t="s">
+      <c r="R7" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="S7" s="21"/>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A8" s="21" t="s">
+      <c r="S7" s="9"/>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A8" s="9" t="s">
         <v>63</v>
       </c>
       <c r="B8" t="s">
@@ -3066,13 +3098,13 @@
       <c r="C8" t="s">
         <v>68</v>
       </c>
-      <c r="D8" s="21">
+      <c r="D8" s="9">
         <v>10434</v>
       </c>
-      <c r="E8" s="33">
+      <c r="E8" s="21">
         <v>22920</v>
       </c>
-      <c r="F8" s="8">
+      <c r="F8" s="23">
         <v>9</v>
       </c>
       <c r="G8">
@@ -3090,29 +3122,31 @@
       <c r="K8">
         <v>95</v>
       </c>
-      <c r="L8" s="23">
+      <c r="L8" s="11">
         <v>123933</v>
       </c>
-      <c r="M8" s="19"/>
-      <c r="N8" s="23">
+      <c r="M8" s="11">
+        <v>87010</v>
+      </c>
+      <c r="N8" s="11">
         <v>4109</v>
       </c>
-      <c r="O8" s="21">
+      <c r="O8" s="9">
         <v>3.6</v>
       </c>
-      <c r="P8" s="23" t="s">
+      <c r="P8" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="Q8" s="10" t="s">
+      <c r="Q8" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="R8" s="10" t="s">
+      <c r="R8" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="S8" s="21"/>
-    </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A9" s="21" t="s">
+      <c r="S8" s="9"/>
+    </row>
+    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A9" s="9" t="s">
         <v>71</v>
       </c>
       <c r="B9" t="s">
@@ -3121,13 +3155,13 @@
       <c r="C9" t="s">
         <v>68</v>
       </c>
-      <c r="D9" s="21">
+      <c r="D9" s="9">
         <v>13166</v>
       </c>
-      <c r="E9" s="33">
+      <c r="E9" s="21">
         <v>13803</v>
       </c>
-      <c r="F9" s="8">
+      <c r="F9" s="23">
         <v>6</v>
       </c>
       <c r="G9">
@@ -3145,29 +3179,31 @@
       <c r="K9">
         <v>95</v>
       </c>
-      <c r="L9" s="23">
+      <c r="L9" s="11">
         <v>205412</v>
       </c>
-      <c r="M9" s="19"/>
-      <c r="N9" s="23">
+      <c r="M9" s="11">
+        <v>145128</v>
+      </c>
+      <c r="N9" s="11">
         <v>2635</v>
       </c>
-      <c r="O9" s="21">
+      <c r="O9" s="9">
         <v>1.4</v>
       </c>
-      <c r="P9" s="23" t="s">
+      <c r="P9" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="Q9" s="10" t="s">
+      <c r="Q9" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="R9" s="10" t="s">
+      <c r="R9" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="S9" s="21"/>
-    </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
-      <c r="A10" s="21" t="s">
+      <c r="S9" s="9"/>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A10" s="9" t="s">
         <v>73</v>
       </c>
       <c r="B10" t="s">
@@ -3176,13 +3212,13 @@
       <c r="C10" t="s">
         <v>68</v>
       </c>
-      <c r="D10" s="21">
+      <c r="D10" s="9">
         <v>13289</v>
       </c>
-      <c r="E10" s="33">
+      <c r="E10" s="21">
         <v>13126</v>
       </c>
-      <c r="F10" s="8">
+      <c r="F10" s="23">
         <v>8</v>
       </c>
       <c r="G10">
@@ -3200,751 +3236,863 @@
       <c r="K10">
         <v>96</v>
       </c>
-      <c r="L10" s="23">
+      <c r="L10" s="11">
         <v>193682</v>
       </c>
-      <c r="M10" s="19"/>
-      <c r="N10" s="23">
+      <c r="M10" s="11">
+        <v>135986</v>
+      </c>
+      <c r="N10" s="11">
         <v>2465</v>
       </c>
-      <c r="O10" s="21">
+      <c r="O10" s="9">
         <v>1.4</v>
       </c>
-      <c r="P10" s="23" t="s">
+      <c r="P10" s="11" t="s">
         <v>97</v>
       </c>
-      <c r="Q10" s="10" t="s">
+      <c r="Q10" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="R10" s="10" t="s">
+      <c r="R10" s="24" t="s">
         <v>98</v>
       </c>
-      <c r="S10" s="21"/>
-    </row>
-    <row r="11" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A11" s="21"/>
-      <c r="D11" s="21"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="22"/>
-      <c r="G11" s="21"/>
-      <c r="H11" s="21"/>
-      <c r="I11" s="23"/>
-      <c r="J11" s="24"/>
-      <c r="K11" s="21"/>
-      <c r="L11" s="23"/>
-      <c r="M11" s="23"/>
-      <c r="N11" s="23"/>
-      <c r="O11" s="21"/>
-      <c r="P11" s="23"/>
-      <c r="Q11" s="26" t="s">
+      <c r="S10" s="9"/>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A11" s="9"/>
+      <c r="D11" s="9"/>
+      <c r="E11" s="21"/>
+      <c r="F11" s="10"/>
+      <c r="G11" s="9"/>
+      <c r="H11" s="9"/>
+      <c r="I11" s="11"/>
+      <c r="J11" s="12"/>
+      <c r="K11" s="9"/>
+      <c r="L11" s="11"/>
+      <c r="M11" s="14" t="s">
         <v>116</v>
       </c>
-      <c r="R11" s="26"/>
-      <c r="S11" s="21"/>
-    </row>
-    <row r="12" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A12" s="21"/>
-      <c r="D12" s="21"/>
-      <c r="E12" s="33"/>
-      <c r="F12" s="22"/>
-      <c r="G12" s="21"/>
-      <c r="H12" s="21"/>
-      <c r="I12" s="23"/>
-      <c r="J12" s="24"/>
-      <c r="K12" s="21"/>
-      <c r="L12" s="23"/>
-      <c r="M12" s="23"/>
-      <c r="N12" s="23"/>
-      <c r="O12" s="21"/>
-      <c r="P12" s="23"/>
-      <c r="Q12" s="26" t="s">
-        <v>117</v>
-      </c>
-      <c r="R12" s="21"/>
-      <c r="S12" s="21"/>
-    </row>
-    <row r="13" spans="1:19" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A13" s="21"/>
-      <c r="D13" s="21"/>
-      <c r="E13" s="33"/>
-      <c r="F13" s="36" t="s">
+      <c r="N11" s="11"/>
+      <c r="O11" s="9"/>
+      <c r="P11" s="11"/>
+      <c r="Q11" s="14" t="s">
+        <v>112</v>
+      </c>
+      <c r="R11" s="14"/>
+      <c r="S11" s="9"/>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A12" s="9"/>
+      <c r="D12" s="9"/>
+      <c r="E12" s="21"/>
+      <c r="F12" s="10"/>
+      <c r="G12" s="9"/>
+      <c r="H12" s="9"/>
+      <c r="I12" s="11"/>
+      <c r="J12" s="12"/>
+      <c r="K12" s="9"/>
+      <c r="L12" s="11"/>
+      <c r="M12" s="11"/>
+      <c r="N12" s="11"/>
+      <c r="O12" s="9"/>
+      <c r="P12" s="11"/>
+      <c r="Q12" s="14" t="s">
+        <v>113</v>
+      </c>
+      <c r="R12" s="9"/>
+      <c r="S12" s="9"/>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A13" s="9"/>
+      <c r="D13" s="9"/>
+      <c r="E13" s="21"/>
+      <c r="F13" s="10"/>
+      <c r="G13" s="9"/>
+      <c r="H13" s="9"/>
+      <c r="I13" s="11"/>
+      <c r="J13" s="12"/>
+      <c r="K13" s="9"/>
+      <c r="L13" s="11"/>
+      <c r="M13" s="11"/>
+      <c r="N13" s="11"/>
+      <c r="O13" s="9"/>
+      <c r="P13" s="11"/>
+      <c r="Q13" s="14"/>
+      <c r="R13" s="9"/>
+      <c r="S13" s="9"/>
+    </row>
+    <row r="14" spans="1:19" ht="38.4" customHeight="1" x14ac:dyDescent="0.35">
+      <c r="A14" s="9"/>
+      <c r="D14" s="9"/>
+      <c r="E14" s="21"/>
+      <c r="F14" s="31" t="s">
         <v>99</v>
       </c>
-      <c r="G13" s="35"/>
-      <c r="H13" s="35"/>
-      <c r="I13" s="35"/>
-      <c r="J13" s="35"/>
-      <c r="K13" s="35"/>
-      <c r="L13" s="16" t="s">
+      <c r="G14" s="32"/>
+      <c r="H14" s="32"/>
+      <c r="I14" s="32"/>
+      <c r="J14" s="32"/>
+      <c r="K14" s="32"/>
+      <c r="L14" s="33" t="s">
+        <v>115</v>
+      </c>
+      <c r="M14" s="33"/>
+      <c r="N14" s="33"/>
+      <c r="O14" s="33"/>
+      <c r="P14" s="33"/>
+      <c r="Q14" s="14"/>
+      <c r="R14" s="14"/>
+      <c r="S14" s="9"/>
+    </row>
+    <row r="15" spans="1:19" ht="61.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A15" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="9"/>
+      <c r="E15" s="20"/>
+      <c r="F15" s="16" t="s">
+        <v>110</v>
+      </c>
+      <c r="G15" s="17"/>
+      <c r="H15" s="17"/>
+      <c r="I15" s="18"/>
+      <c r="J15" s="16"/>
+      <c r="K15" s="17"/>
+      <c r="L15" s="16" t="s">
+        <v>102</v>
+      </c>
+      <c r="M15" s="16" t="s">
         <v>118</v>
       </c>
-      <c r="M13" s="16"/>
-      <c r="N13" s="16"/>
-      <c r="O13" s="16"/>
-      <c r="P13" s="16"/>
-      <c r="Q13" s="26"/>
-      <c r="R13" s="26"/>
-      <c r="S13" s="21"/>
-    </row>
-    <row r="14" spans="1:19" s="11" customFormat="1" ht="61.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A14" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D14" s="21"/>
-      <c r="E14" s="32"/>
-      <c r="F14" s="28" t="s">
+      <c r="N15" s="16" t="s">
+        <v>119</v>
+      </c>
+      <c r="O15" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="P15" s="16" t="s">
         <v>114</v>
       </c>
-      <c r="G14" s="29"/>
-      <c r="H14" s="29"/>
-      <c r="I14" s="30"/>
-      <c r="J14" s="28"/>
-      <c r="K14" s="29"/>
-      <c r="L14" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="M14" s="28" t="s">
+      <c r="Q15" s="12"/>
+      <c r="R15" s="12"/>
+      <c r="S15" s="9"/>
+    </row>
+    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A16" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D16" s="9"/>
+      <c r="E16" s="21"/>
+      <c r="F16" s="7">
+        <v>185</v>
+      </c>
+      <c r="G16" s="9"/>
+      <c r="H16" s="9"/>
+      <c r="I16" s="11"/>
+      <c r="J16" s="12"/>
+      <c r="K16" s="9"/>
+      <c r="L16" s="11">
+        <v>48464</v>
+      </c>
+      <c r="M16" s="11">
+        <v>32964</v>
+      </c>
+      <c r="N16" s="11">
+        <v>3641</v>
+      </c>
+      <c r="O16" s="15">
+        <f>N16/M16</f>
+        <v>0.1104538284188812</v>
+      </c>
+      <c r="P16" s="22">
+        <f>F16/N16</f>
+        <v>5.0810216973358968E-2</v>
+      </c>
+      <c r="Q16" s="14"/>
+      <c r="R16" s="14"/>
+      <c r="S16" s="9"/>
+    </row>
+    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A17" s="9" t="s">
+        <v>77</v>
+      </c>
+      <c r="D17" s="9"/>
+      <c r="E17" s="21"/>
+      <c r="F17" s="7">
+        <v>85</v>
+      </c>
+      <c r="G17" s="9"/>
+      <c r="H17" s="9"/>
+      <c r="I17" s="11"/>
+      <c r="J17" s="12"/>
+      <c r="K17" s="9"/>
+      <c r="L17" s="11">
+        <v>52822</v>
+      </c>
+      <c r="M17" s="11">
+        <v>35392</v>
+      </c>
+      <c r="N17" s="11">
+        <v>2699</v>
+      </c>
+      <c r="O17" s="15">
+        <f t="shared" ref="O17:O18" si="0">N17/M17</f>
+        <v>7.6260171790235087E-2</v>
+      </c>
+      <c r="P17" s="22">
+        <f t="shared" ref="P17:P22" si="1">F17/N17</f>
+        <v>3.1493145609484997E-2</v>
+      </c>
+      <c r="Q17" s="14"/>
+      <c r="R17" s="14"/>
+      <c r="S17" s="9"/>
+    </row>
+    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A18" s="9" t="s">
+        <v>79</v>
+      </c>
+      <c r="D18" s="9"/>
+      <c r="E18" s="21"/>
+      <c r="F18" s="7">
+        <v>43</v>
+      </c>
+      <c r="G18" s="9"/>
+      <c r="H18" s="9"/>
+      <c r="I18" s="11"/>
+      <c r="J18" s="12"/>
+      <c r="K18" s="9"/>
+      <c r="L18" s="11">
+        <v>45706</v>
+      </c>
+      <c r="M18" s="11">
+        <v>29810</v>
+      </c>
+      <c r="N18" s="11">
+        <v>1638</v>
+      </c>
+      <c r="O18" s="15">
+        <f t="shared" si="0"/>
+        <v>5.4948004025494802E-2</v>
+      </c>
+      <c r="P18" s="22">
+        <f t="shared" si="1"/>
+        <v>2.6251526251526252E-2</v>
+      </c>
+      <c r="Q18" s="34" t="s">
+        <v>122</v>
+      </c>
+      <c r="R18" s="14"/>
+      <c r="S18" s="9"/>
+    </row>
+    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A19" s="9"/>
+      <c r="D19" s="9"/>
+      <c r="E19" s="21"/>
+      <c r="F19" s="10"/>
+      <c r="G19" s="9"/>
+      <c r="H19" s="9"/>
+      <c r="I19" s="11"/>
+      <c r="J19" s="12"/>
+      <c r="K19" s="9"/>
+      <c r="L19" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="M19" s="34">
+        <f>AVERAGE(M16:M18)</f>
+        <v>32722</v>
+      </c>
+      <c r="N19" s="35">
+        <f>AVERAGE(N16:N18)</f>
+        <v>2659.3333333333335</v>
+      </c>
+      <c r="O19" s="36">
+        <f t="shared" ref="O19:P19" si="2">AVERAGE(O16:O18)</f>
+        <v>8.0554001411537027E-2</v>
+      </c>
+      <c r="P19" s="36">
+        <f t="shared" si="2"/>
+        <v>3.6184962944790074E-2</v>
+      </c>
+      <c r="Q19" s="37">
+        <f>P19*O19</f>
+        <v>2.9148435561310347E-3</v>
+      </c>
+      <c r="R19" s="14"/>
+      <c r="S19" s="9"/>
+    </row>
+    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A20" s="9" t="s">
+        <v>63</v>
+      </c>
+      <c r="D20" s="9"/>
+      <c r="E20" s="21"/>
+      <c r="F20" s="7">
+        <v>1695</v>
+      </c>
+      <c r="G20" s="9"/>
+      <c r="H20" s="9"/>
+      <c r="I20" s="11"/>
+      <c r="J20" s="12"/>
+      <c r="K20" s="9"/>
+      <c r="L20" s="9">
+        <v>39792</v>
+      </c>
+      <c r="M20" s="9">
+        <v>27902</v>
+      </c>
+      <c r="N20" s="9">
+        <v>5946</v>
+      </c>
+      <c r="O20" s="15">
+        <f>N20/M20</f>
+        <v>0.21310300336893412</v>
+      </c>
+      <c r="P20" s="22">
+        <f>F20/N20</f>
+        <v>0.28506559031281536</v>
+      </c>
+      <c r="Q20" s="34"/>
+      <c r="R20" s="14"/>
+      <c r="S20" s="9"/>
+    </row>
+    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A21" s="9" t="s">
+        <v>71</v>
+      </c>
+      <c r="D21" s="9"/>
+      <c r="E21" s="21"/>
+      <c r="F21" s="7">
+        <v>395</v>
+      </c>
+      <c r="G21" s="9"/>
+      <c r="H21" s="9"/>
+      <c r="I21" s="11"/>
+      <c r="J21" s="12"/>
+      <c r="K21" s="9"/>
+      <c r="L21" s="9">
+        <v>54769</v>
+      </c>
+      <c r="M21" s="11">
+        <v>39791</v>
+      </c>
+      <c r="N21" s="11">
+        <v>3736</v>
+      </c>
+      <c r="O21" s="15">
+        <f t="shared" ref="O21:O22" si="3">N21/M21</f>
+        <v>9.389057827146842E-2</v>
+      </c>
+      <c r="P21" s="22">
+        <f t="shared" si="1"/>
+        <v>0.10572805139186295</v>
+      </c>
+      <c r="Q21" s="34"/>
+      <c r="R21" s="14"/>
+      <c r="S21" s="9"/>
+    </row>
+    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A22" s="9" t="s">
+        <v>73</v>
+      </c>
+      <c r="D22" s="9"/>
+      <c r="E22" s="21"/>
+      <c r="F22" s="7">
+        <v>301</v>
+      </c>
+      <c r="G22" s="9"/>
+      <c r="H22" s="9"/>
+      <c r="I22" s="11"/>
+      <c r="J22" s="12"/>
+      <c r="K22" s="9"/>
+      <c r="L22" s="11">
+        <v>51594</v>
+      </c>
+      <c r="M22" s="11">
+        <v>34727</v>
+      </c>
+      <c r="N22" s="11">
+        <v>3452</v>
+      </c>
+      <c r="O22" s="15">
+        <f t="shared" si="3"/>
+        <v>9.9403922020330007E-2</v>
+      </c>
+      <c r="P22" s="22">
+        <f t="shared" si="1"/>
+        <v>8.7195828505214373E-2</v>
+      </c>
+      <c r="Q22" s="34"/>
+      <c r="R22" s="14"/>
+      <c r="S22" s="9"/>
+    </row>
+    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A23" s="9"/>
+      <c r="D23" s="9"/>
+      <c r="E23" s="21"/>
+      <c r="F23" s="10"/>
+      <c r="G23" s="9"/>
+      <c r="H23" s="9"/>
+      <c r="I23" s="11"/>
+      <c r="J23" s="12"/>
+      <c r="K23" s="9"/>
+      <c r="L23" s="34" t="s">
+        <v>121</v>
+      </c>
+      <c r="M23" s="34">
+        <f>AVERAGE(M20:M22)</f>
+        <v>34140</v>
+      </c>
+      <c r="N23" s="34">
+        <f>AVERAGE(N20:N22)</f>
+        <v>4378</v>
+      </c>
+      <c r="O23" s="36">
+        <f t="shared" ref="O23" si="4">AVERAGE(O20:O22)</f>
+        <v>0.1354658345535775</v>
+      </c>
+      <c r="P23" s="36">
+        <f>AVERAGE(P20:P22)</f>
+        <v>0.15932982340329757</v>
+      </c>
+      <c r="Q23" s="37">
+        <f>P23*O23</f>
+        <v>2.1583747496601829E-2</v>
+      </c>
+      <c r="R23" s="14"/>
+      <c r="S23" s="9"/>
+    </row>
+    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A24" s="9"/>
+      <c r="D24" s="9"/>
+      <c r="E24" s="21"/>
+      <c r="F24" s="10"/>
+      <c r="G24" s="9"/>
+      <c r="H24" s="9"/>
+      <c r="I24" s="11"/>
+      <c r="J24" s="12"/>
+      <c r="K24" s="9"/>
+      <c r="L24" s="34"/>
+      <c r="M24" s="34"/>
+      <c r="N24" s="34"/>
+      <c r="O24" s="36"/>
+      <c r="P24" s="36"/>
+      <c r="Q24" s="14"/>
+      <c r="R24" s="14"/>
+      <c r="S24" s="9"/>
+    </row>
+    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A25" s="9"/>
+      <c r="D25" s="9"/>
+      <c r="E25" s="21"/>
+      <c r="F25" s="10"/>
+      <c r="G25" s="9"/>
+      <c r="H25" s="9"/>
+      <c r="I25" s="11"/>
+      <c r="J25" s="12"/>
+      <c r="K25" s="9"/>
+      <c r="L25" s="11"/>
+      <c r="M25" s="11"/>
+      <c r="N25" s="11"/>
+      <c r="O25" s="9"/>
+      <c r="P25" s="26" t="s">
+        <v>111</v>
+      </c>
+      <c r="Q25" s="26"/>
+      <c r="R25" s="26"/>
+      <c r="S25" s="9"/>
+    </row>
+    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A26" s="9"/>
+      <c r="D26" s="9"/>
+      <c r="E26" s="21"/>
+      <c r="F26" s="10"/>
+      <c r="I26" s="4"/>
+      <c r="J26" s="3"/>
+      <c r="M26" s="27" t="s">
+        <v>95</v>
+      </c>
+      <c r="N26" s="27"/>
+      <c r="O26" s="27"/>
+      <c r="P26" s="27"/>
+      <c r="Q26" s="27"/>
+      <c r="R26" s="27"/>
+      <c r="S26" s="9"/>
+    </row>
+    <row r="27" spans="1:19" ht="46.5" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A27" s="10" t="s">
+        <v>0</v>
+      </c>
+      <c r="D27" s="9"/>
+      <c r="E27" s="21"/>
+      <c r="F27" s="12"/>
+      <c r="G27" s="9"/>
+      <c r="H27" s="9"/>
+      <c r="I27" s="11"/>
+      <c r="J27" s="12"/>
+      <c r="K27" s="9"/>
+      <c r="L27" s="12"/>
+      <c r="M27" s="16" t="s">
+        <v>118</v>
+      </c>
+      <c r="N27" s="16"/>
+      <c r="O27" s="16"/>
+      <c r="P27" s="16" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q27" s="16" t="s">
+        <v>105</v>
+      </c>
+      <c r="R27" s="16" t="s">
+        <v>100</v>
+      </c>
+      <c r="S27" s="12"/>
+    </row>
+    <row r="28" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A28" s="9" t="s">
+        <v>75</v>
+      </c>
+      <c r="D28" s="9"/>
+      <c r="E28" s="21"/>
+      <c r="F28" s="10"/>
+      <c r="G28" s="9"/>
+      <c r="H28" s="9"/>
+      <c r="I28" s="11"/>
+      <c r="J28" s="12"/>
+      <c r="K28" s="9"/>
+      <c r="L28" s="12"/>
+      <c r="M28" s="25" t="s">
+        <v>123</v>
+      </c>
+      <c r="N28" s="12"/>
+      <c r="O28" s="12"/>
+      <c r="P28" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q28" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="R28" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="N14" s="28" t="s">
-        <v>103</v>
-      </c>
-      <c r="O14" s="28" t="s">
-        <v>42</v>
-      </c>
-      <c r="P14" s="28" t="s">
-        <v>119</v>
-      </c>
-      <c r="Q14" s="24"/>
-      <c r="R14" s="24"/>
-      <c r="S14" s="21"/>
-    </row>
-    <row r="15" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A15" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="D15" s="21"/>
-      <c r="E15" s="33"/>
-      <c r="F15" s="15">
-        <v>185</v>
-      </c>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
-      <c r="I15" s="23"/>
-      <c r="J15" s="24"/>
-      <c r="K15" s="21"/>
-      <c r="L15" s="23">
-        <v>48464</v>
-      </c>
-      <c r="M15" s="23">
-        <v>32964</v>
-      </c>
-      <c r="N15" s="23">
-        <v>3641</v>
-      </c>
-      <c r="O15" s="27">
-        <f>N15/L15</f>
-        <v>7.5127930009904254E-2</v>
-      </c>
-      <c r="P15" s="37">
-        <f>F15/N15</f>
-        <v>5.0810216973358968E-2</v>
-      </c>
-      <c r="Q15" s="26"/>
-      <c r="R15" s="26"/>
-      <c r="S15" s="21"/>
-    </row>
-    <row r="16" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A16" s="21" t="s">
+      <c r="S28" s="9"/>
+    </row>
+    <row r="29" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A29" s="9" t="s">
         <v>77</v>
       </c>
-      <c r="D16" s="21"/>
-      <c r="E16" s="33"/>
-      <c r="F16" s="15">
-        <v>85</v>
-      </c>
-      <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
-      <c r="I16" s="23"/>
-      <c r="J16" s="24"/>
-      <c r="K16" s="21"/>
-      <c r="L16" s="23">
-        <v>52822</v>
-      </c>
-      <c r="M16" s="23">
-        <v>35392</v>
-      </c>
-      <c r="N16" s="23">
-        <v>2699</v>
-      </c>
-      <c r="O16" s="27">
-        <f>N16/L16</f>
-        <v>5.1096134186513195E-2</v>
-      </c>
-      <c r="P16" s="37">
-        <f t="shared" ref="P16:P20" si="0">F16/N16</f>
-        <v>3.1493145609484997E-2</v>
-      </c>
-      <c r="Q16" s="26"/>
-      <c r="R16" s="26"/>
-      <c r="S16" s="21"/>
-    </row>
-    <row r="17" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A17" s="21" t="s">
+      <c r="D29" s="9"/>
+      <c r="E29" s="21"/>
+      <c r="F29" s="10"/>
+      <c r="G29" s="9"/>
+      <c r="H29" s="9"/>
+      <c r="I29" s="11"/>
+      <c r="J29" s="12"/>
+      <c r="K29" s="9"/>
+      <c r="L29" s="12"/>
+      <c r="M29" s="25"/>
+      <c r="N29" s="12"/>
+      <c r="O29" s="12"/>
+      <c r="P29" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q29" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="R29" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="S29" s="9"/>
+    </row>
+    <row r="30" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A30" s="9" t="s">
         <v>79</v>
       </c>
-      <c r="D17" s="21"/>
-      <c r="E17" s="33"/>
-      <c r="F17" s="15">
-        <v>43</v>
-      </c>
-      <c r="G17" s="21"/>
-      <c r="H17" s="21"/>
-      <c r="I17" s="23"/>
-      <c r="J17" s="24"/>
-      <c r="K17" s="21"/>
-      <c r="L17" s="23">
-        <v>45706</v>
-      </c>
-      <c r="M17" s="23">
-        <v>29810</v>
-      </c>
-      <c r="N17" s="23">
-        <v>1638</v>
-      </c>
-      <c r="O17" s="27">
-        <f>N17/L17</f>
-        <v>3.5837745591388442E-2</v>
-      </c>
-      <c r="P17" s="37">
-        <f t="shared" si="0"/>
-        <v>2.6251526251526252E-2</v>
-      </c>
-      <c r="Q17" s="26"/>
-      <c r="R17" s="26"/>
-      <c r="S17" s="21"/>
-    </row>
-    <row r="18" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A18" s="21" t="s">
+      <c r="D30" s="9"/>
+      <c r="E30" s="21"/>
+      <c r="F30" s="10"/>
+      <c r="G30" s="9"/>
+      <c r="H30" s="9"/>
+      <c r="I30" s="11"/>
+      <c r="J30" s="12"/>
+      <c r="K30" s="9"/>
+      <c r="L30" s="12"/>
+      <c r="M30" s="25"/>
+      <c r="N30" s="12"/>
+      <c r="O30" s="12"/>
+      <c r="P30" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q30" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="R30" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="S30" s="9"/>
+    </row>
+    <row r="31" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A31" s="9" t="s">
         <v>63</v>
       </c>
-      <c r="D18" s="21"/>
-      <c r="E18" s="33"/>
-      <c r="F18" s="15">
-        <v>1695</v>
-      </c>
-      <c r="G18" s="21"/>
-      <c r="H18" s="21"/>
-      <c r="I18" s="23"/>
-      <c r="J18" s="24"/>
-      <c r="K18" s="21"/>
-      <c r="L18" s="21">
-        <v>39792</v>
-      </c>
-      <c r="M18" s="21">
-        <v>27902</v>
-      </c>
-      <c r="N18" s="21">
-        <v>5946</v>
-      </c>
-      <c r="O18" s="27">
-        <f>N18/L18</f>
-        <v>0.14942702050663451</v>
-      </c>
-      <c r="P18" s="37">
-        <f t="shared" si="0"/>
-        <v>0.28506559031281536</v>
-      </c>
-      <c r="Q18" s="26"/>
-      <c r="R18" s="26"/>
-      <c r="S18" s="21"/>
-    </row>
-    <row r="19" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A19" s="21" t="s">
+      <c r="D31" s="9"/>
+      <c r="E31" s="21"/>
+      <c r="F31" s="10"/>
+      <c r="G31" s="9"/>
+      <c r="H31" s="9"/>
+      <c r="I31" s="11"/>
+      <c r="J31" s="12"/>
+      <c r="K31" s="9"/>
+      <c r="L31" s="12"/>
+      <c r="M31" s="25"/>
+      <c r="N31" s="12"/>
+      <c r="O31" s="12"/>
+      <c r="P31" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q31" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="R31" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="S31" s="9"/>
+    </row>
+    <row r="32" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A32" s="9" t="s">
         <v>71</v>
       </c>
-      <c r="D19" s="21"/>
-      <c r="E19" s="33"/>
-      <c r="F19" s="15">
-        <v>395</v>
-      </c>
-      <c r="G19" s="21"/>
-      <c r="H19" s="21"/>
-      <c r="I19" s="23"/>
-      <c r="J19" s="24"/>
-      <c r="K19" s="21"/>
-      <c r="L19" s="21">
-        <v>54769</v>
-      </c>
-      <c r="M19" s="23">
-        <v>39791</v>
-      </c>
-      <c r="N19" s="23">
-        <v>3736</v>
-      </c>
-      <c r="O19" s="27">
-        <f t="shared" ref="O19:O20" si="1">N19/L19</f>
-        <v>6.8213770563640017E-2</v>
-      </c>
-      <c r="P19" s="37">
-        <f t="shared" si="0"/>
-        <v>0.10572805139186295</v>
-      </c>
-      <c r="Q19" s="26"/>
-      <c r="R19" s="26"/>
-      <c r="S19" s="21"/>
-    </row>
-    <row r="20" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A20" s="21" t="s">
+      <c r="D32" s="9"/>
+      <c r="E32" s="21"/>
+      <c r="F32" s="10"/>
+      <c r="G32" s="9"/>
+      <c r="H32" s="9"/>
+      <c r="I32" s="11"/>
+      <c r="J32" s="12"/>
+      <c r="K32" s="9"/>
+      <c r="L32" s="12"/>
+      <c r="M32" s="25"/>
+      <c r="N32" s="12"/>
+      <c r="O32" s="12"/>
+      <c r="P32" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q32" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="R32" s="8" t="s">
+        <v>104</v>
+      </c>
+      <c r="S32" s="9"/>
+    </row>
+    <row r="33" spans="1:19" ht="15" customHeight="1" x14ac:dyDescent="0.3">
+      <c r="A33" s="9" t="s">
         <v>73</v>
       </c>
-      <c r="D20" s="21"/>
-      <c r="E20" s="33"/>
-      <c r="F20" s="15">
-        <v>301</v>
-      </c>
-      <c r="G20" s="21"/>
-      <c r="H20" s="21"/>
-      <c r="I20" s="23"/>
-      <c r="J20" s="24"/>
-      <c r="K20" s="21"/>
-      <c r="L20" s="23">
-        <v>51594</v>
-      </c>
-      <c r="M20" s="23">
-        <v>34727</v>
-      </c>
-      <c r="N20" s="23">
-        <v>3452</v>
-      </c>
-      <c r="O20" s="27">
-        <f t="shared" si="1"/>
-        <v>6.6907004690467883E-2</v>
-      </c>
-      <c r="P20" s="37">
-        <f t="shared" si="0"/>
-        <v>8.7195828505214373E-2</v>
-      </c>
-      <c r="Q20" s="26"/>
-      <c r="R20" s="26"/>
-      <c r="S20" s="21"/>
-    </row>
-    <row r="21" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A21" s="21"/>
-      <c r="D21" s="21"/>
-      <c r="E21" s="33"/>
-      <c r="F21" s="22"/>
-      <c r="G21" s="21"/>
-      <c r="H21" s="21"/>
-      <c r="I21" s="23"/>
-      <c r="J21" s="24"/>
-      <c r="K21" s="21"/>
-      <c r="L21" s="23"/>
-      <c r="M21" s="23"/>
-      <c r="N21" s="23"/>
-      <c r="O21" s="21"/>
-      <c r="P21" s="34" t="s">
-        <v>115</v>
-      </c>
-      <c r="Q21" s="34"/>
-      <c r="R21" s="34"/>
-      <c r="S21" s="21"/>
-    </row>
-    <row r="22" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A22" s="21"/>
-      <c r="D22" s="21"/>
-      <c r="E22" s="33"/>
-      <c r="F22" s="22"/>
-      <c r="I22" s="5"/>
-      <c r="J22" s="13"/>
-      <c r="L22" s="9" t="s">
-        <v>95</v>
-      </c>
-      <c r="M22" s="9"/>
-      <c r="N22" s="9"/>
-      <c r="O22" s="9"/>
-      <c r="P22" s="9"/>
-      <c r="Q22" s="9"/>
-      <c r="R22" s="9"/>
-      <c r="S22" s="21"/>
-    </row>
-    <row r="23" spans="1:19" s="11" customFormat="1" ht="46.5" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A23" s="22" t="s">
-        <v>0</v>
-      </c>
-      <c r="D23" s="21"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="24"/>
-      <c r="G23" s="21"/>
-      <c r="H23" s="21"/>
-      <c r="I23" s="23"/>
-      <c r="J23" s="24"/>
-      <c r="K23" s="21"/>
-      <c r="L23" s="28" t="s">
-        <v>102</v>
-      </c>
-      <c r="M23" s="28" t="s">
+      <c r="D33" s="9"/>
+      <c r="E33" s="21"/>
+      <c r="F33" s="10"/>
+      <c r="G33" s="9"/>
+      <c r="H33" s="9"/>
+      <c r="I33" s="11"/>
+      <c r="J33" s="12"/>
+      <c r="K33" s="9"/>
+      <c r="L33" s="12"/>
+      <c r="M33" s="25"/>
+      <c r="N33" s="12"/>
+      <c r="O33" s="12"/>
+      <c r="P33" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="Q33" s="8" t="s">
+        <v>107</v>
+      </c>
+      <c r="R33" s="8" t="s">
         <v>104</v>
       </c>
-      <c r="N23" s="28"/>
-      <c r="O23" s="28"/>
-      <c r="P23" s="28" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q23" s="28" t="s">
-        <v>107</v>
-      </c>
-      <c r="R23" s="28" t="s">
-        <v>100</v>
-      </c>
-      <c r="S23" s="24"/>
-    </row>
-    <row r="24" spans="1:19" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A24" s="21" t="s">
-        <v>75</v>
-      </c>
-      <c r="D24" s="21"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="22"/>
-      <c r="G24" s="21"/>
-      <c r="H24" s="21"/>
-      <c r="I24" s="23"/>
-      <c r="J24" s="24"/>
-      <c r="K24" s="21"/>
-      <c r="L24" s="24"/>
-      <c r="M24" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="N24" s="24"/>
-      <c r="O24" s="24"/>
-      <c r="P24" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q24" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="R24" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="S24" s="21"/>
-    </row>
-    <row r="25" spans="1:19" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A25" s="21" t="s">
-        <v>77</v>
-      </c>
-      <c r="D25" s="21"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="22"/>
-      <c r="G25" s="21"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="23"/>
-      <c r="J25" s="24"/>
-      <c r="K25" s="21"/>
-      <c r="L25" s="24"/>
-      <c r="M25" s="20"/>
-      <c r="N25" s="24"/>
-      <c r="O25" s="24"/>
-      <c r="P25" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q25" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="R25" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="S25" s="21"/>
-    </row>
-    <row r="26" spans="1:19" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A26" s="21" t="s">
-        <v>79</v>
-      </c>
-      <c r="D26" s="21"/>
-      <c r="E26" s="33"/>
-      <c r="F26" s="22"/>
-      <c r="G26" s="21"/>
-      <c r="H26" s="21"/>
-      <c r="I26" s="23"/>
-      <c r="J26" s="24"/>
-      <c r="K26" s="21"/>
-      <c r="L26" s="24"/>
-      <c r="M26" s="20"/>
-      <c r="N26" s="24"/>
-      <c r="O26" s="24"/>
-      <c r="P26" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q26" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="R26" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="S26" s="21"/>
-    </row>
-    <row r="27" spans="1:19" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="21" t="s">
-        <v>63</v>
-      </c>
-      <c r="D27" s="21"/>
-      <c r="E27" s="33"/>
-      <c r="F27" s="22"/>
-      <c r="G27" s="21"/>
-      <c r="H27" s="21"/>
-      <c r="I27" s="23"/>
-      <c r="J27" s="24"/>
-      <c r="K27" s="21"/>
-      <c r="L27" s="24"/>
-      <c r="M27" s="20"/>
-      <c r="N27" s="24"/>
-      <c r="O27" s="24"/>
-      <c r="P27" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q27" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="R27" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="S27" s="21"/>
-    </row>
-    <row r="28" spans="1:19" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A28" s="21" t="s">
-        <v>71</v>
-      </c>
-      <c r="D28" s="21"/>
-      <c r="E28" s="33"/>
-      <c r="F28" s="22"/>
-      <c r="G28" s="21"/>
-      <c r="H28" s="21"/>
-      <c r="I28" s="23"/>
-      <c r="J28" s="24"/>
-      <c r="K28" s="21"/>
-      <c r="L28" s="24"/>
-      <c r="M28" s="20"/>
-      <c r="N28" s="24"/>
-      <c r="O28" s="24"/>
-      <c r="P28" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q28" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="R28" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="S28" s="21"/>
-    </row>
-    <row r="29" spans="1:19" s="11" customFormat="1" ht="15" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A29" s="21" t="s">
-        <v>73</v>
-      </c>
-      <c r="D29" s="21"/>
-      <c r="E29" s="33"/>
-      <c r="F29" s="22"/>
-      <c r="G29" s="21"/>
-      <c r="H29" s="21"/>
-      <c r="I29" s="23"/>
-      <c r="J29" s="24"/>
-      <c r="K29" s="21"/>
-      <c r="L29" s="24"/>
-      <c r="M29" s="20"/>
-      <c r="N29" s="24"/>
-      <c r="O29" s="24"/>
-      <c r="P29" s="24" t="s">
-        <v>98</v>
-      </c>
-      <c r="Q29" s="18" t="s">
-        <v>110</v>
-      </c>
-      <c r="R29" s="18" t="s">
-        <v>106</v>
-      </c>
-      <c r="S29" s="21"/>
-    </row>
-    <row r="30" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="A30" s="21"/>
-      <c r="D30" s="21"/>
-      <c r="E30" s="21"/>
-      <c r="F30" s="22"/>
-      <c r="G30" s="21"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="23"/>
-      <c r="J30" s="24"/>
-      <c r="K30" s="21"/>
-      <c r="L30" s="23"/>
-      <c r="M30" s="23"/>
-      <c r="N30" s="23"/>
-      <c r="O30" s="21"/>
-      <c r="P30" s="23"/>
-      <c r="Q30" s="26"/>
-      <c r="R30" s="26"/>
-      <c r="S30" s="21"/>
-    </row>
-    <row r="31" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F31" s="12"/>
-      <c r="I31" s="5"/>
-      <c r="J31" s="13"/>
-      <c r="L31" s="5"/>
-      <c r="M31" s="5"/>
-      <c r="N31" s="5"/>
-      <c r="P31" s="5"/>
-      <c r="Q31" s="14"/>
-      <c r="R31" s="14"/>
-      <c r="S31" s="21"/>
-    </row>
-    <row r="32" spans="1:19" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F32" s="12"/>
-      <c r="I32" s="5"/>
-      <c r="J32" s="13"/>
-      <c r="L32" s="5"/>
-      <c r="M32" s="5"/>
-      <c r="N32" s="5"/>
-      <c r="P32" s="5"/>
-      <c r="Q32" s="14"/>
-      <c r="R32" s="14"/>
-    </row>
-    <row r="33" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F33" s="12"/>
-      <c r="I33" s="5"/>
-      <c r="J33" s="13"/>
-      <c r="L33" s="5"/>
-      <c r="M33" s="5"/>
-      <c r="N33" s="5"/>
-      <c r="P33" s="5"/>
-      <c r="Q33" s="14"/>
-      <c r="R33" s="14"/>
-    </row>
-    <row r="34" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F34" s="12"/>
-      <c r="I34" s="5"/>
-      <c r="J34" s="13"/>
-      <c r="L34" s="5"/>
-      <c r="M34" s="5"/>
-      <c r="N34" s="5"/>
-      <c r="P34" s="5"/>
+      <c r="S33" s="9"/>
+    </row>
+    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A34" s="9"/>
+      <c r="D34" s="9"/>
+      <c r="E34" s="9"/>
+      <c r="F34" s="10"/>
+      <c r="G34" s="9"/>
+      <c r="H34" s="9"/>
+      <c r="I34" s="11"/>
+      <c r="J34" s="12"/>
+      <c r="K34" s="9"/>
+      <c r="L34" s="11"/>
+      <c r="M34" s="11"/>
+      <c r="N34" s="11"/>
+      <c r="O34" s="9"/>
+      <c r="P34" s="11"/>
       <c r="Q34" s="14"/>
       <c r="R34" s="14"/>
-    </row>
-    <row r="35" spans="1:18" s="11" customFormat="1" x14ac:dyDescent="0.25">
-      <c r="F35" s="12"/>
-      <c r="I35" s="5"/>
-      <c r="J35" s="13"/>
-      <c r="L35" s="5"/>
-      <c r="M35" s="5"/>
-      <c r="N35" s="5"/>
-      <c r="P35" s="5"/>
-      <c r="Q35" s="14"/>
-      <c r="R35" s="14"/>
-    </row>
-    <row r="36" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="B36" t="s">
+      <c r="S34" s="9"/>
+    </row>
+    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="F35" s="5"/>
+      <c r="I35" s="4"/>
+      <c r="J35" s="3"/>
+      <c r="L35" s="4"/>
+      <c r="M35" s="4"/>
+      <c r="N35" s="4"/>
+      <c r="P35" s="4"/>
+      <c r="Q35" s="6"/>
+      <c r="R35" s="6"/>
+      <c r="S35" s="9"/>
+    </row>
+    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="F36" s="5"/>
+      <c r="I36" s="4"/>
+      <c r="J36" s="3"/>
+      <c r="L36" s="4"/>
+      <c r="M36" s="4"/>
+      <c r="N36" s="4"/>
+      <c r="P36" s="4"/>
+      <c r="Q36" s="6"/>
+      <c r="R36" s="6"/>
+    </row>
+    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="F37" s="5"/>
+      <c r="I37" s="4"/>
+      <c r="J37" s="3"/>
+      <c r="L37" s="4"/>
+      <c r="M37" s="4"/>
+      <c r="N37" s="4"/>
+      <c r="P37" s="4"/>
+      <c r="Q37" s="6"/>
+      <c r="R37" s="6"/>
+    </row>
+    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="F38" s="5"/>
+      <c r="I38" s="4"/>
+      <c r="J38" s="3"/>
+      <c r="L38" s="4"/>
+      <c r="M38" s="4"/>
+      <c r="N38" s="4"/>
+      <c r="P38" s="4"/>
+      <c r="Q38" s="6"/>
+      <c r="R38" s="6"/>
+    </row>
+    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="F39" s="5"/>
+      <c r="I39" s="4"/>
+      <c r="J39" s="3"/>
+      <c r="L39" s="4"/>
+      <c r="M39" s="4"/>
+      <c r="N39" s="4"/>
+      <c r="P39" s="4"/>
+      <c r="Q39" s="6"/>
+      <c r="R39" s="6"/>
+    </row>
+    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="B40" t="s">
         <v>82</v>
       </c>
-      <c r="C36" t="s">
+      <c r="C40" t="s">
         <v>82</v>
       </c>
-      <c r="D36" t="s">
+      <c r="D40" t="s">
         <v>82</v>
       </c>
-      <c r="E36" t="s">
+      <c r="E40" t="s">
         <v>82</v>
       </c>
-      <c r="F36" t="s">
+      <c r="F40" t="s">
         <v>82</v>
       </c>
-      <c r="G36" t="s">
+      <c r="G40" t="s">
         <v>82</v>
       </c>
-      <c r="H36" t="s">
+      <c r="H40" t="s">
         <v>82</v>
       </c>
-      <c r="I36" t="s">
+      <c r="I40" t="s">
         <v>82</v>
       </c>
-      <c r="J36" t="s">
+      <c r="J40" t="s">
         <v>82</v>
       </c>
-      <c r="K36" t="s">
+      <c r="K40" t="s">
         <v>82</v>
       </c>
-      <c r="L36" t="s">
+      <c r="L40" t="s">
         <v>82</v>
       </c>
-      <c r="N36" t="s">
+      <c r="N40" t="s">
         <v>82</v>
       </c>
-      <c r="O36" t="s">
+      <c r="O40" t="s">
         <v>82</v>
       </c>
     </row>
-    <row r="37" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="L37" t="s">
+    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="L41" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="39" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
         <v>85</v>
       </c>
     </row>
-    <row r="40" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
         <v>86</v>
       </c>
     </row>
-    <row r="41" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
+    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="42" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A42" t="s">
+    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
         <v>88</v>
       </c>
     </row>
-    <row r="43" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A43" t="s">
+    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="44" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A44" t="s">
+    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="45" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A45" t="s">
+    <row r="49" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>91</v>
       </c>
     </row>
-    <row r="46" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A46" t="s">
+    <row r="50" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="47" spans="1:18" x14ac:dyDescent="0.25">
-      <c r="A47" t="s">
+    <row r="51" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
         <v>93</v>
       </c>
     </row>
-    <row r="49" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A49" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
         <v>94</v>
       </c>
     </row>
   </sheetData>
-  <mergeCells count="9">
-    <mergeCell ref="M24:M29"/>
-    <mergeCell ref="M5:M10"/>
-    <mergeCell ref="P2:R2"/>
-    <mergeCell ref="P21:R21"/>
-    <mergeCell ref="L13:P13"/>
-    <mergeCell ref="L22:R22"/>
-    <mergeCell ref="P3:R3"/>
+  <mergeCells count="8">
     <mergeCell ref="D3:E3"/>
     <mergeCell ref="F3:O3"/>
+    <mergeCell ref="M28:M33"/>
+    <mergeCell ref="P2:R2"/>
+    <mergeCell ref="P25:R25"/>
+    <mergeCell ref="L14:P14"/>
+    <mergeCell ref="P3:R3"/>
+    <mergeCell ref="M26:R26"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>